<commit_message>
updated logboek & removed unneeded docx
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26894237-A7ED-426A-A900-C27A677F064D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A5B1FE-9876-4ED8-8329-0FB65FC752CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Database desgin</t>
+  </si>
+  <si>
+    <t>Updated read me en converted briefing</t>
   </si>
 </sst>
 </file>
@@ -661,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,11 +786,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C462,J5,D5:D48)</f>
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1087,10 +1090,18 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="2">
+        <v>44103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1">
+        <v>30</v>
+      </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -7107,6 +7118,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7238,15 +7258,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
@@ -7264,6 +7275,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7279,12 +7298,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
query SSMS of visual studio toegevoegd + logboek
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Json reader to List&lt;Strip&gt; aangemaakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">query aanpassen en converten en testen MYSQQL -&gt; SSMS </t>
   </si>
 </sst>
 </file>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L881"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,11 +742,11 @@
       </c>
       <c r="K3" s="1">
         <f ca="1">SUMIF(C3:C460,J3,D3:D46)</f>
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>6.25</v>
+        <v>6.583333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1140,10 +1143,18 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1">
+        <v>20</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -7139,15 +7150,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7279,6 +7281,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
@@ -7296,14 +7307,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7319,4 +7322,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Use case strip tonen
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ciki3\Desktop\SCHOOL 20-21\Projectwerk\projectwerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar\Documents\School\Projectwerk\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E4294-44C3-4B20-8517-A526AC5F3982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="765" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="840" yWindow="255" windowWidth="28020" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -114,11 +115,17 @@
   <si>
     <t xml:space="preserve">query aanpassen en converten en testen MYSQQL -&gt; SSMS </t>
   </si>
+  <si>
+    <t>Use cases aanmaken</t>
+  </si>
+  <si>
+    <t>Use cases verder afwerken</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,7 +365,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -669,11 +676,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L881"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="1">
-        <f ca="1">SUMIF(C3:C460,J3,D3:D46)</f>
+        <f ca="1">SUMIF(C3:C461,J3,D3:D47)</f>
         <v>395</v>
       </c>
       <c r="L3" s="6">
@@ -767,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="1">
-        <f ca="1">SUMIF(C4:C461,J4,D4:D47)</f>
+        <f ca="1">SUMIF(C4:C462,J4,D4:D48)</f>
         <v>290</v>
       </c>
       <c r="L4" s="6">
@@ -793,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="1">
-        <f ca="1">SUMIF(C5:C462,J5,D5:D48)</f>
+        <f ca="1">SUMIF(C5:C463,J5,D5:D49)</f>
         <v>520</v>
       </c>
       <c r="L5" s="6">
@@ -819,12 +826,12 @@
         <v>12</v>
       </c>
       <c r="K6" s="10">
-        <f ca="1">SUMIF(C6:C463,J6,D6:D49)</f>
-        <v>270</v>
+        <f ca="1">SUMIF(C6:C464,J6,D6:D50)</f>
+        <v>360</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1132,13 +1139,13 @@
         <v>44104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -1147,28 +1154,44 @@
         <v>44104</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="1">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1">
         <v>20</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1">
+        <v>30</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -7128,13 +7151,20 @@
       <c r="D881" s="1"/>
       <c r="E881" s="1"/>
     </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A882" s="1"/>
+      <c r="B882" s="1"/>
+      <c r="C882" s="1"/>
+      <c r="D882" s="1"/>
+      <c r="E882" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C881">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C882" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$J$3:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -7144,9 +7174,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7282,26 +7315,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7325,9 +7347,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
JSON reader + logboek
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar\Documents\School\Projectwerk\projectwerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ciki3\Desktop\SCHOOL 20-21\Projectwerk\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D67D79-6042-4651-BD93-7369D6D584A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="315" windowWidth="27675" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="315" windowWidth="27675" windowHeight="15420"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -145,11 +144,17 @@
   <si>
     <t>DbFuncties aanpassen + maken</t>
   </si>
+  <si>
+    <t>Json reader to List&lt;Strip&gt; aanpassen naar nieuwe bestand</t>
+  </si>
+  <si>
+    <t>klasses en hun constructers aanpassen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,7 +394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -700,11 +705,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L882"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,11 +778,11 @@
       </c>
       <c r="K3" s="1">
         <f ca="1">SUMIF(C3:C461,J3,D3:D47)</f>
-        <v>590</v>
+        <v>665</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>9.8333333333333339</v>
+        <v>11.083333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1384,17 +1389,33 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="A42" s="2">
+        <v>44115</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1">
+        <v>60</v>
+      </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="A43" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="1">
+        <v>15</v>
+      </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -7276,7 +7297,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C882" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C882">
       <formula1>$J$3:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -7295,12 +7316,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7432,6 +7447,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
@@ -7441,22 +7462,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7472,4 +7477,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added time from initial rework see ree branch
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70990e190d1d57a3/scool/projectwerk/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="114_{625D20F3-5FA0-4F3F-9B1C-56E58D2E2483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{292840A3-97F4-4905-AD9D-0673ED890740}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42711DD7-7EE9-4EC9-B215-27C663A823B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23016" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>FindAllByReeks/Uitgeverij gemaakt en gedebugged</t>
+  </si>
+  <si>
+    <t>rebuild project</t>
   </si>
 </sst>
 </file>
@@ -740,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L885"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,11 +865,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C466,J5,D5:D49)</f>
-        <v>1040</v>
+        <v>1175</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>17.333333333333332</v>
+        <v>19.583333333333332</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1766,10 +1769,18 @@
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="A65" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1">
+        <v>135</v>
+      </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -7660,18 +7671,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7693,6 +7704,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7706,12 +7725,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated log after rework step 1
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42711DD7-7EE9-4EC9-B215-27C663A823B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D81A90-DBC3-42D6-ACFE-3A4DEDBFBAC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L885"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
@@ -865,11 +865,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C466,J5,D5:D49)</f>
-        <v>1175</v>
+        <v>1200</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19.583333333333332</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1779,7 +1779,7 @@
         <v>11</v>
       </c>
       <c r="D65" s="1">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -7671,18 +7671,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7704,14 +7704,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7725,4 +7717,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cleaned up project and git
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B36746D-2FC3-4D88-8289-4555B7DD6498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884F058C-AE25-47DE-B2A7-35739DA9B00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>fixing app config, writing en testing strip update</t>
+  </si>
+  <si>
+    <t>clean up solution + git</t>
   </si>
 </sst>
 </file>
@@ -769,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,11 +894,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C467,J5,D5:D49)</f>
-        <v>2060</v>
+        <v>2070</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>34.333333333333336</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2170,10 +2173,18 @@
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
+      <c r="A90" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="1">
+        <v>10</v>
+      </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -7773,12 +7784,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7910,6 +7915,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
@@ -7919,22 +7930,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7950,4 +7945,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GUI search by id + logboek
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="68">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>GUI sorteer aanmaken, code correcties in GUI, opmaken uitproberen</t>
+  </si>
+  <si>
+    <t>GUI strip vinden op id + opmaken uitproberen en knoppen functies correcteren in GUI</t>
   </si>
 </sst>
 </file>
@@ -792,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,11 +865,11 @@
       </c>
       <c r="K3" s="1">
         <f ca="1">SUMIF(C3:C465,J3,D3:D47)</f>
-        <v>1515</v>
+        <v>1575</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>25.25</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2328,10 +2331,18 @@
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+      <c r="A99" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="1">
+        <v>60</v>
+      </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -7868,6 +7879,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -7999,12 +8016,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
@@ -8014,6 +8025,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8029,20 +8056,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding tests and debugging stripaddtest -> test doesn't run idk why
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60055F3A-00EF-4628-A9A6-74C1E6AD4F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADA2137-9EAC-47E7-950D-5219156AC43A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="72">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Provided testing classes for models + cleaning unneeded branches</t>
+  </si>
+  <si>
+    <t>Writing and debugging strip add intigration test</t>
   </si>
 </sst>
 </file>
@@ -806,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,11 +931,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C467,J5,D5:D49)</f>
-        <v>2660</v>
+        <v>2690</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>44.333333333333336</v>
+        <v>44.833333333333336</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2462,10 +2465,18 @@
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="A107" s="2">
+        <v>44141</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" s="1">
+        <v>30</v>
+      </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
LOGBOEK+ comboboxen in gui
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="79">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Coding uitleg/discussie session discord</t>
+  </si>
+  <si>
+    <t>Progressbar in JSON UI laten werken</t>
+  </si>
+  <si>
+    <t>Reeks/uitgeverij tetbox vervangen door combo boxen, strip toevoegen laten werken en testen</t>
   </si>
 </sst>
 </file>
@@ -823,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L886"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,11 +899,11 @@
       </c>
       <c r="K3" s="1">
         <f ca="1">SUMIF(C3:C465,J3,D3:D47)</f>
-        <v>2030</v>
+        <v>2140</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>33.833333333333336</v>
+        <v>35.666666666666664</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2704,17 +2710,33 @@
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
+      <c r="A122" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="1">
+        <v>75</v>
+      </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+      <c r="A123" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="1">
+        <v>35</v>
+      </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -8080,6 +8102,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -8211,15 +8242,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
@@ -8237,6 +8259,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8252,12 +8282,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
repository place holder, model +conv
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5304AB92-D131-493E-B444-24B20B3CD7B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5647C-C1CE-4041-AE04-4BE4B0EB86E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="99">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Aanzet impact md</t>
+  </si>
+  <si>
+    <t>Model + repos</t>
   </si>
 </sst>
 </file>
@@ -888,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L887"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,11 +1013,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C468,J5,D5:D49)</f>
-        <v>4138</v>
+        <v>4203</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>68.966666666666669</v>
+        <v>70.05</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3369,10 +3372,18 @@
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
+      <c r="A162" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" s="1">
+        <v>65</v>
+      </c>
       <c r="E162" s="1"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -8466,21 +8477,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -8612,10 +8608,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8637,19 +8658,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated with missing time
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F775CCF2-BF73-4983-A242-12E0BD876434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B9C41E-8B97-4B71-9FF1-8D08F4735E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="111">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Debugging gitignore</t>
+  </si>
+  <si>
+    <t>Voorbereiden meeting</t>
+  </si>
+  <si>
+    <t>Meeting voorbereiden</t>
   </si>
 </sst>
 </file>
@@ -918,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L888"/>
+  <dimension ref="A1:L917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="H180" sqref="H180"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="F195" sqref="F195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,12 +995,12 @@
         <v>9</v>
       </c>
       <c r="K3" s="1">
-        <f ca="1">SUMIF(C3:C467,J3,D3:D47)</f>
-        <v>3105</v>
+        <f ca="1">SUMIF(C3:C496,J3,D3:D61)</f>
+        <v>3285</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>51.75</v>
+        <v>54.75</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1015,12 +1021,12 @@
         <v>10</v>
       </c>
       <c r="K4" s="1">
-        <f ca="1">SUMIF(C4:C468,J4,D4:D48)</f>
-        <v>2620</v>
+        <f ca="1">SUMIF(C4:C497,J4,D4:D62)</f>
+        <v>2800</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" ref="L4:L6" ca="1" si="0">K4/60</f>
-        <v>43.666666666666664</v>
+        <v>46.666666666666664</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1041,12 +1047,12 @@
         <v>11</v>
       </c>
       <c r="K5" s="1">
-        <f ca="1">SUMIF(C5:C469,J5,D5:D49)</f>
-        <v>4763</v>
+        <f ca="1">SUMIF(C5:C498,J5,D5:D63)</f>
+        <v>5588</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>79.38333333333334</v>
+        <v>93.13333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1067,12 +1073,12 @@
         <v>12</v>
       </c>
       <c r="K6" s="10">
-        <f ca="1">SUMIF(C6:C470,J6,D6:D50)</f>
-        <v>2525</v>
+        <f ca="1">SUMIF(C6:C499,J6,D6:D64)</f>
+        <v>2705</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>42.083333333333336</v>
+        <v>45.083333333333336</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1230,13 +1236,13 @@
         <v>44099</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -1248,7 +1254,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1">
         <v>45</v>
@@ -1263,7 +1269,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1">
         <v>45</v>
@@ -1272,16 +1278,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>44102</v>
+        <v>44099</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1290,13 +1296,13 @@
         <v>44102</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1308,7 +1314,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1">
         <v>60</v>
@@ -1323,7 +1329,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1">
         <v>60</v>
@@ -1332,31 +1338,31 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>44103</v>
+        <v>44102</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>44103</v>
+        <v>44102</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1365,43 +1371,43 @@
         <v>44103</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="1">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>44104</v>
+        <v>44103</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>44104</v>
+        <v>44103</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1410,175 +1416,175 @@
         <v>44104</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D29" s="1">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>44105</v>
+        <v>44104</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D30" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>44106</v>
+        <v>44104</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>44106</v>
+        <v>44105</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1">
         <v>30</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="1">
-        <v>210</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>44107</v>
+        <v>44105</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>44108</v>
+        <v>44105</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D34" s="1">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>44109</v>
+        <v>44105</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D35" s="1">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>44109</v>
+        <v>44105</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>44109</v>
+        <v>44105</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>44109</v>
+        <v>44106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D38" s="1">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>44109</v>
+        <v>44106</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1">
-        <v>80</v>
+        <v>210</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>44112</v>
+        <v>44107</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" s="1">
         <v>60</v>
@@ -1587,397 +1593,397 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>44112</v>
+        <v>44108</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="1">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>44115</v>
+        <v>44109</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D42" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>44116</v>
+        <v>44109</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>44116</v>
+        <v>44109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="1">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>44117</v>
+        <v>44109</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45" s="1">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>44117</v>
+        <v>44109</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D46" s="1">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>44117</v>
+        <v>44109</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D47" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>44117</v>
+        <v>44112</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>44117</v>
+        <v>44112</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D49" s="1">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>44117</v>
+        <v>44112</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" s="1">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>44119</v>
+        <v>44112</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D51" s="1">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>44120</v>
+        <v>44112</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D52" s="1">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>44120</v>
+        <v>44112</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D53" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>44120</v>
+        <v>44112</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D54" s="1">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>44120</v>
+        <v>44115</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D55" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>44120</v>
+        <v>44116</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="1">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>44122</v>
+        <v>44116</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>44122</v>
+        <v>44117</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D58" s="1">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>44122</v>
+        <v>44117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D59" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>44122</v>
+        <v>44117</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>44123</v>
+        <v>44117</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>44123</v>
+        <v>44117</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="1">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>44123</v>
+        <v>44117</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D63" s="1">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>44123</v>
+        <v>44117</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D64" s="1">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>44123</v>
+        <v>44119</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D65" s="1">
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>44126</v>
+        <v>44120</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="1">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>44126</v>
+        <v>44120</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>41</v>
@@ -1986,13 +1992,13 @@
         <v>9</v>
       </c>
       <c r="D67" s="1">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>44126</v>
+        <v>44120</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>41</v>
@@ -2001,13 +2007,13 @@
         <v>10</v>
       </c>
       <c r="D68" s="1">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>44126</v>
+        <v>44120</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>41</v>
@@ -2016,13 +2022,13 @@
         <v>11</v>
       </c>
       <c r="D69" s="1">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>44126</v>
+        <v>44120</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>41</v>
@@ -2031,133 +2037,133 @@
         <v>12</v>
       </c>
       <c r="D70" s="1">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>44127</v>
+        <v>44120</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D71" s="1">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>44130</v>
+        <v>44122</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D72" s="1">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>44130</v>
+        <v>44122</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D73" s="1">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>44130</v>
+        <v>44122</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D74" s="1">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>44130</v>
+        <v>44122</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D75" s="1">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>44130</v>
+        <v>44123</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D76" s="1">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>44130</v>
+        <v>44123</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D77" s="1">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>44130</v>
+        <v>44123</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D78" s="1">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>44133</v>
+        <v>44123</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>33</v>
@@ -2166,13 +2172,13 @@
         <v>9</v>
       </c>
       <c r="D79" s="1">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>44133</v>
+        <v>44123</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>33</v>
@@ -2181,124 +2187,124 @@
         <v>10</v>
       </c>
       <c r="D80" s="1">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>44133</v>
+        <v>44123</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D81" s="1">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>44133</v>
+        <v>44126</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D82" s="1">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>44136</v>
+        <v>44126</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D83" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>44136</v>
+        <v>44126</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D84" s="1">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>44137</v>
+        <v>44126</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D85" s="1">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>44137</v>
+        <v>44126</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D86" s="1">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>44137</v>
+        <v>44126</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D87" s="1">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>44137</v>
+        <v>44127</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88" s="1">
         <v>120</v>
@@ -2307,163 +2313,163 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D89" s="1">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D90" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D91" s="1">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D92" s="1">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="1">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D94" s="1">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D95" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>44138</v>
+        <v>44130</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D96" s="1">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>44139</v>
+        <v>44133</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="1">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>44139</v>
+        <v>44133</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D98" s="1">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>44140</v>
+        <v>44133</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D99" s="1">
         <v>60</v>
@@ -2472,328 +2478,328 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>44140</v>
+        <v>44133</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D100" s="1">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>44140</v>
+        <v>44133</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D101" s="1">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>44140</v>
+        <v>44136</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D102" s="1">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>44140</v>
+        <v>44136</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D103" s="1">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>44140</v>
+        <v>44137</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D104" s="1">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>44141</v>
+        <v>44137</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D105" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>44141</v>
+        <v>44137</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D106" s="1">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>44141</v>
+        <v>44137</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D107" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>44144</v>
+        <v>44137</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D108" s="1">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>44145</v>
+        <v>44138</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D109" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>44145</v>
+        <v>44138</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D110" s="1">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>44145</v>
+        <v>44138</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D111" s="1">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>44145</v>
+        <v>44138</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D112" s="1">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>44145</v>
+        <v>44138</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D113" s="1">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>44146</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C114" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D114" s="12">
-        <v>45</v>
+        <v>44138</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="1">
+        <v>120</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>44147</v>
+        <v>44138</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D115" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>44147</v>
+        <v>44138</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D116" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>44147</v>
+        <v>44139</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D117" s="1">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>44148</v>
+        <v>44139</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D118" s="1">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>44148</v>
+        <v>44140</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D119" s="1">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>44148</v>
+        <v>44140</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D120" s="1">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>44148</v>
+        <v>44140</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D121" s="1">
         <v>105</v>
@@ -2802,133 +2808,133 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>44148</v>
+        <v>44140</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D122" s="1">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="13">
-        <v>44148</v>
-      </c>
-      <c r="B123" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D123" s="12">
-        <v>75</v>
+      <c r="A123" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="1">
+        <v>105</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>44149</v>
+        <v>44140</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D124" s="1">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>44150</v>
+        <v>44140</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D125" s="1">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>44151</v>
+        <v>44141</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D126" s="1">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>44151</v>
+        <v>44141</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D127" s="1">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>44151</v>
+        <v>44141</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D128" s="1">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>44151</v>
+        <v>44144</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D129" s="1">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>44152</v>
+        <v>44145</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D130" s="1">
         <v>30</v>
@@ -2937,103 +2943,103 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>44153</v>
+        <v>44145</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D131" s="1">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>44153</v>
+        <v>44145</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D132" s="1">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>44153</v>
+        <v>44145</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D133" s="1">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>44153</v>
+        <v>44145</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D134" s="1">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>44155</v>
+        <v>44145</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D135" s="1">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>44155</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D136" s="1">
-        <v>30</v>
+        <v>44146</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" s="12">
+        <v>45</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>44155</v>
+        <v>44147</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D137" s="1">
         <v>30</v>
@@ -3042,163 +3048,163 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>44155</v>
+        <v>44147</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D138" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>44158</v>
+        <v>44147</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D139" s="1">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>44158</v>
+        <v>44148</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D140" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>44158</v>
+        <v>44148</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D141" s="1">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>44158</v>
+        <v>44148</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D142" s="1">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>44158</v>
+        <v>44148</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D143" s="1">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>44160</v>
+        <v>44148</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D144" s="1">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>44160</v>
+        <v>44148</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D145" s="1">
-        <v>240</v>
+        <v>75</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
-        <v>44160</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D146" s="1">
-        <v>110</v>
+      <c r="A146" s="13">
+        <v>44148</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" s="12">
+        <v>75</v>
       </c>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>44161</v>
+        <v>44149</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D147" s="1">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>44162</v>
+        <v>44150</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D148" s="1">
         <v>90</v>
@@ -3207,328 +3213,328 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>44162</v>
+        <v>44151</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D149" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>44162</v>
+        <v>44151</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D150" s="1">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>44162</v>
+        <v>44151</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D151" s="1">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>44162</v>
+        <v>44151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D152" s="1">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>44165</v>
+        <v>44151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D153" s="1">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>44165</v>
+        <v>44152</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D154" s="1">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>44165</v>
+        <v>44153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D155" s="1">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>44165</v>
+        <v>44153</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D156" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>44165</v>
+        <v>44153</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D157" s="1">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>44165</v>
+        <v>44153</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D158" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>44165</v>
+        <v>44155</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D159" s="1">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E159" s="1"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>44165</v>
+        <v>44155</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D160" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>44165</v>
+        <v>44155</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D161" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>44165</v>
+        <v>44155</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D162" s="1">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="E162" s="1"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>44165</v>
+        <v>44155</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D163" s="1">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E163" s="1"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>44165</v>
+        <v>44158</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D164" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>44165</v>
+        <v>44158</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D165" s="1">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>44165</v>
+        <v>44158</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D166" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E166" s="1"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>44165</v>
+        <v>44158</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D167" s="1">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>44166</v>
+        <v>44158</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D168" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E168" s="1"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>44166</v>
+        <v>44158</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D169" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E169" s="1"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>44167</v>
+        <v>44160</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D170" s="1">
         <v>60</v>
@@ -3537,58 +3543,58 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>44167</v>
+        <v>44160</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D171" s="1">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="E171" s="1"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>44167</v>
+        <v>44160</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D172" s="1">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>44167</v>
+        <v>44161</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D173" s="1">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D174" s="1">
         <v>90</v>
@@ -3597,58 +3603,58 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D175" s="1">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E175" s="1"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D176" s="1">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D177" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>44167</v>
+        <v>44162</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D178" s="1">
         <v>45</v>
@@ -3656,206 +3662,438 @@
       <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-      <c r="D179" s="1"/>
+      <c r="A179" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D179" s="1">
+        <v>45</v>
+      </c>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
-      <c r="D180" s="1"/>
+      <c r="A180" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D180" s="1">
+        <v>5</v>
+      </c>
       <c r="E180" s="1"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
+      <c r="A181" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D181" s="1">
+        <v>180</v>
+      </c>
       <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
-      <c r="C182" s="1"/>
-      <c r="D182" s="1"/>
+      <c r="A182" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" s="1">
+        <v>30</v>
+      </c>
       <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
-      <c r="C183" s="1"/>
-      <c r="D183" s="1"/>
+      <c r="A183" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" s="1">
+        <v>120</v>
+      </c>
       <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
-      <c r="D184" s="1"/>
+      <c r="A184" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" s="1">
+        <v>120</v>
+      </c>
       <c r="E184" s="1"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
-      <c r="C185" s="1"/>
-      <c r="D185" s="1"/>
+      <c r="A185" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D185" s="1">
+        <v>120</v>
+      </c>
       <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
-      <c r="C186" s="1"/>
-      <c r="D186" s="1"/>
+      <c r="A186" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D186" s="1">
+        <v>120</v>
+      </c>
       <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
-      <c r="D187" s="1"/>
+      <c r="A187" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" s="1">
+        <v>38</v>
+      </c>
       <c r="E187" s="1"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
-      <c r="C188" s="1"/>
-      <c r="D188" s="1"/>
+      <c r="A188" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D188" s="1">
+        <v>15</v>
+      </c>
       <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
-      <c r="D189" s="1"/>
+      <c r="A189" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" s="1">
+        <v>20</v>
+      </c>
       <c r="E189" s="1"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
-      <c r="D190" s="1"/>
+      <c r="A190" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" s="1">
+        <v>65</v>
+      </c>
       <c r="E190" s="1"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
-      <c r="C191" s="1"/>
-      <c r="D191" s="1"/>
+      <c r="A191" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" s="1">
+        <v>20</v>
+      </c>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-      <c r="B192" s="1"/>
-      <c r="C192" s="1"/>
-      <c r="D192" s="1"/>
+      <c r="A192" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D192" s="1">
+        <v>100</v>
+      </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
-      <c r="B193" s="1"/>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1"/>
+      <c r="A193" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" s="1">
+        <v>120</v>
+      </c>
       <c r="E193" s="1"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-      <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
-      <c r="D194" s="1"/>
+      <c r="A194" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" s="1">
+        <v>70</v>
+      </c>
       <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1"/>
+      <c r="A195" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="1">
+        <v>15</v>
+      </c>
       <c r="E195" s="1"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-      <c r="B196" s="1"/>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1"/>
+      <c r="A196" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D196" s="1">
+        <v>90</v>
+      </c>
       <c r="E196" s="1"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
-      <c r="B197" s="1"/>
-      <c r="C197" s="1"/>
-      <c r="D197" s="1"/>
+      <c r="A197" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D197" s="1">
+        <v>90</v>
+      </c>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
-      <c r="B198" s="1"/>
-      <c r="C198" s="1"/>
-      <c r="D198" s="1"/>
+      <c r="A198" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D198" s="1">
+        <v>60</v>
+      </c>
       <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="1"/>
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
-      <c r="D199" s="1"/>
+      <c r="A199" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D199" s="1">
+        <v>30</v>
+      </c>
       <c r="E199" s="1"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1"/>
+      <c r="A200" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D200" s="1">
+        <v>90</v>
+      </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="1"/>
-      <c r="B201" s="1"/>
-      <c r="C201" s="1"/>
-      <c r="D201" s="1"/>
+      <c r="A201" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D201" s="1">
+        <v>90</v>
+      </c>
       <c r="E201" s="1"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="1"/>
-      <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
-      <c r="D202" s="1"/>
+      <c r="A202" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D202" s="1">
+        <v>90</v>
+      </c>
       <c r="E202" s="1"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="1"/>
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
-      <c r="D203" s="1"/>
+      <c r="A203" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D203" s="1">
+        <v>90</v>
+      </c>
       <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="1"/>
-      <c r="B204" s="1"/>
-      <c r="C204" s="1"/>
-      <c r="D204" s="1"/>
+      <c r="A204" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D204" s="1">
+        <v>70</v>
+      </c>
       <c r="E204" s="1"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" s="1"/>
-      <c r="B205" s="1"/>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1"/>
+      <c r="A205" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D205" s="1">
+        <v>70</v>
+      </c>
       <c r="E205" s="1"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="1"/>
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1"/>
+      <c r="A206" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D206" s="1">
+        <v>40</v>
+      </c>
       <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
-      <c r="C207" s="1"/>
-      <c r="D207" s="1"/>
+      <c r="A207" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D207" s="1">
+        <v>45</v>
+      </c>
       <c r="E207" s="1"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -8625,13 +8863,216 @@
       <c r="D888" s="1"/>
       <c r="E888" s="1"/>
     </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A889" s="1"/>
+      <c r="B889" s="1"/>
+      <c r="C889" s="1"/>
+      <c r="D889" s="1"/>
+      <c r="E889" s="1"/>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A890" s="1"/>
+      <c r="B890" s="1"/>
+      <c r="C890" s="1"/>
+      <c r="D890" s="1"/>
+      <c r="E890" s="1"/>
+    </row>
+    <row r="891" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A891" s="1"/>
+      <c r="B891" s="1"/>
+      <c r="C891" s="1"/>
+      <c r="D891" s="1"/>
+      <c r="E891" s="1"/>
+    </row>
+    <row r="892" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A892" s="1"/>
+      <c r="B892" s="1"/>
+      <c r="C892" s="1"/>
+      <c r="D892" s="1"/>
+      <c r="E892" s="1"/>
+    </row>
+    <row r="893" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A893" s="1"/>
+      <c r="B893" s="1"/>
+      <c r="C893" s="1"/>
+      <c r="D893" s="1"/>
+      <c r="E893" s="1"/>
+    </row>
+    <row r="894" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A894" s="1"/>
+      <c r="B894" s="1"/>
+      <c r="C894" s="1"/>
+      <c r="D894" s="1"/>
+      <c r="E894" s="1"/>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A895" s="1"/>
+      <c r="B895" s="1"/>
+      <c r="C895" s="1"/>
+      <c r="D895" s="1"/>
+      <c r="E895" s="1"/>
+    </row>
+    <row r="896" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A896" s="1"/>
+      <c r="B896" s="1"/>
+      <c r="C896" s="1"/>
+      <c r="D896" s="1"/>
+      <c r="E896" s="1"/>
+    </row>
+    <row r="897" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A897" s="1"/>
+      <c r="B897" s="1"/>
+      <c r="C897" s="1"/>
+      <c r="D897" s="1"/>
+      <c r="E897" s="1"/>
+    </row>
+    <row r="898" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A898" s="1"/>
+      <c r="B898" s="1"/>
+      <c r="C898" s="1"/>
+      <c r="D898" s="1"/>
+      <c r="E898" s="1"/>
+    </row>
+    <row r="899" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A899" s="1"/>
+      <c r="B899" s="1"/>
+      <c r="C899" s="1"/>
+      <c r="D899" s="1"/>
+      <c r="E899" s="1"/>
+    </row>
+    <row r="900" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A900" s="1"/>
+      <c r="B900" s="1"/>
+      <c r="C900" s="1"/>
+      <c r="D900" s="1"/>
+      <c r="E900" s="1"/>
+    </row>
+    <row r="901" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A901" s="1"/>
+      <c r="B901" s="1"/>
+      <c r="C901" s="1"/>
+      <c r="D901" s="1"/>
+      <c r="E901" s="1"/>
+    </row>
+    <row r="902" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A902" s="1"/>
+      <c r="B902" s="1"/>
+      <c r="C902" s="1"/>
+      <c r="D902" s="1"/>
+      <c r="E902" s="1"/>
+    </row>
+    <row r="903" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A903" s="1"/>
+      <c r="B903" s="1"/>
+      <c r="C903" s="1"/>
+      <c r="D903" s="1"/>
+      <c r="E903" s="1"/>
+    </row>
+    <row r="904" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A904" s="1"/>
+      <c r="B904" s="1"/>
+      <c r="C904" s="1"/>
+      <c r="D904" s="1"/>
+      <c r="E904" s="1"/>
+    </row>
+    <row r="905" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A905" s="1"/>
+      <c r="B905" s="1"/>
+      <c r="C905" s="1"/>
+      <c r="D905" s="1"/>
+      <c r="E905" s="1"/>
+    </row>
+    <row r="906" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A906" s="1"/>
+      <c r="B906" s="1"/>
+      <c r="C906" s="1"/>
+      <c r="D906" s="1"/>
+      <c r="E906" s="1"/>
+    </row>
+    <row r="907" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A907" s="1"/>
+      <c r="B907" s="1"/>
+      <c r="C907" s="1"/>
+      <c r="D907" s="1"/>
+      <c r="E907" s="1"/>
+    </row>
+    <row r="908" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A908" s="1"/>
+      <c r="B908" s="1"/>
+      <c r="C908" s="1"/>
+      <c r="D908" s="1"/>
+      <c r="E908" s="1"/>
+    </row>
+    <row r="909" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A909" s="1"/>
+      <c r="B909" s="1"/>
+      <c r="C909" s="1"/>
+      <c r="D909" s="1"/>
+      <c r="E909" s="1"/>
+    </row>
+    <row r="910" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A910" s="1"/>
+      <c r="B910" s="1"/>
+      <c r="C910" s="1"/>
+      <c r="D910" s="1"/>
+      <c r="E910" s="1"/>
+    </row>
+    <row r="911" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A911" s="1"/>
+      <c r="B911" s="1"/>
+      <c r="C911" s="1"/>
+      <c r="D911" s="1"/>
+      <c r="E911" s="1"/>
+    </row>
+    <row r="912" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A912" s="1"/>
+      <c r="B912" s="1"/>
+      <c r="C912" s="1"/>
+      <c r="D912" s="1"/>
+      <c r="E912" s="1"/>
+    </row>
+    <row r="913" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A913" s="1"/>
+      <c r="B913" s="1"/>
+      <c r="C913" s="1"/>
+      <c r="D913" s="1"/>
+      <c r="E913" s="1"/>
+    </row>
+    <row r="914" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A914" s="1"/>
+      <c r="B914" s="1"/>
+      <c r="C914" s="1"/>
+      <c r="D914" s="1"/>
+      <c r="E914" s="1"/>
+    </row>
+    <row r="915" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A915" s="1"/>
+      <c r="B915" s="1"/>
+      <c r="C915" s="1"/>
+      <c r="D915" s="1"/>
+      <c r="E915" s="1"/>
+    </row>
+    <row r="916" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A916" s="1"/>
+      <c r="B916" s="1"/>
+      <c r="C916" s="1"/>
+      <c r="D916" s="1"/>
+      <c r="E916" s="1"/>
+    </row>
+    <row r="917" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A917" s="1"/>
+      <c r="B917" s="1"/>
+      <c r="C917" s="1"/>
+      <c r="D917" s="1"/>
+      <c r="E917" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C113 C115:C122 C124:C888" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C147:C917 C137:C145 C3:C135" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$J$3:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -8641,21 +9082,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -8787,31 +9213,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8827,4 +9244,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edit Strip collection wpf + code
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ciki3\Desktop\SCHOOL 20-21\Projectwerk\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E426502-B7C7-4B03-A605-826005D2533D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="116">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -375,12 +374,18 @@
   </si>
   <si>
     <t>Feedback md</t>
+  </si>
+  <si>
+    <t>Edit stripCollection wpf window + code</t>
+  </si>
+  <si>
+    <t>Try catchers in repository</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -932,11 +937,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L917"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L918"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B210" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J218" sqref="J218"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H215" sqref="H215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,12 +1009,12 @@
         <v>9</v>
       </c>
       <c r="K3" s="1">
-        <f ca="1">SUMIF(C3:C496,J3,D3:D61)</f>
-        <v>3365</v>
+        <f ca="1">SUMIF(C3:C497,J3,D3:D61)</f>
+        <v>3470</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>56.083333333333336</v>
+        <v>57.833333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1030,7 +1035,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="1">
-        <f ca="1">SUMIF(C4:C497,J4,D4:D62)</f>
+        <f ca="1">SUMIF(C4:C498,J4,D4:D62)</f>
         <v>2880</v>
       </c>
       <c r="L4" s="6">
@@ -1056,7 +1061,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="1">
-        <f ca="1">SUMIF(C5:C498,J5,D5:D63)</f>
+        <f ca="1">SUMIF(C5:C499,J5,D5:D63)</f>
         <v>5673</v>
       </c>
       <c r="L5" s="6">
@@ -1082,7 +1087,7 @@
         <v>12</v>
       </c>
       <c r="K6" s="10">
-        <f ca="1">SUMIF(C6:C499,J6,D6:D64)</f>
+        <f ca="1">SUMIF(C6:C500,J6,D6:D64)</f>
         <v>2890</v>
       </c>
       <c r="L6" s="8">
@@ -4107,16 +4112,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>44168</v>
+        <v>44167</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D208" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E208" s="1"/>
     </row>
@@ -4125,13 +4130,13 @@
         <v>44168</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D209" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E209" s="1"/>
     </row>
@@ -4140,10 +4145,10 @@
         <v>44168</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D210" s="1">
         <v>80</v>
@@ -4155,10 +4160,10 @@
         <v>44168</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D211" s="1">
         <v>80</v>
@@ -4173,7 +4178,7 @@
         <v>85</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D212" s="1">
         <v>80</v>
@@ -4185,13 +4190,13 @@
         <v>44168</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D213" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E213" s="1"/>
     </row>
@@ -4200,28 +4205,44 @@
         <v>44168</v>
       </c>
       <c r="B214" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D214" s="1">
+        <v>45</v>
+      </c>
+      <c r="E214" s="1"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="C215" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D214" s="1">
+      <c r="D215" s="1">
         <v>5</v>
       </c>
-      <c r="E214" s="1"/>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="1"/>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
-      <c r="D215" s="1"/>
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="1"/>
-      <c r="B216" s="1"/>
-      <c r="C216" s="1"/>
-      <c r="D216" s="1"/>
+      <c r="A216" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D216" s="1">
+        <v>60</v>
+      </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -9131,13 +9152,20 @@
       <c r="D917" s="1"/>
       <c r="E917" s="1"/>
     </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A918" s="1"/>
+      <c r="B918" s="1"/>
+      <c r="C918" s="1"/>
+      <c r="D918" s="1"/>
+      <c r="E918" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C135 C137:C145 C147:C917" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C135 C137:C145 C147:C918">
       <formula1>$J$3:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -9156,6 +9184,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -9287,12 +9321,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
@@ -9302,6 +9330,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9317,20 +9361,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
step in the right direction
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B786B3DF-E081-410A-B97B-C6B4858539D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117EE0D-B99C-448A-8FC6-904394B16DD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="118">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>debugging</t>
+  </si>
+  <si>
+    <t>Debugging StripCollection getall</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K212" sqref="K212"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H223" sqref="H223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,11 +1069,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C498,J5,D5:D63)</f>
-        <v>5863</v>
+        <v>5905</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>97.716666666666669</v>
+        <v>98.416666666666671</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4325,10 +4328,18 @@
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="1"/>
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1"/>
+      <c r="A222" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D222" s="1">
+        <v>42</v>
+      </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -9212,6 +9223,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -9343,22 +9369,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9374,28 +9409,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GUI + JSON GUI + Logboek
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Desktop\repos\projectwerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ciki3\Desktop\SCHOOL 20-21\Projectwerk\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F439B880-9EB3-47D1-946D-B37A110703DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="122">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -390,12 +389,21 @@
   </si>
   <si>
     <t>Fixing getAll stripCollection to get strips</t>
+  </si>
+  <si>
+    <t>JSON gui code aanpassen + GUI mainwindow changes voor collectie</t>
+  </si>
+  <si>
+    <t>12/0/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI aanpassingen om zoektermen te verbeteren </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -947,11 +955,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L917"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L918"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D216" sqref="D216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,12 +1027,12 @@
         <v>9</v>
       </c>
       <c r="K3" s="1">
-        <f ca="1">SUMIF(C3:C496,J3,D3:D61)</f>
-        <v>3505</v>
+        <f ca="1">SUMIF(C3:C497,J3,D3:D61)</f>
+        <v>3540</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">K3/60</f>
-        <v>58.416666666666664</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1045,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="1">
-        <f ca="1">SUMIF(C4:C497,J4,D4:D62)</f>
+        <f ca="1">SUMIF(C4:C498,J4,D4:D62)</f>
         <v>3140</v>
       </c>
       <c r="L4" s="6">
@@ -1071,12 +1079,12 @@
         <v>11</v>
       </c>
       <c r="K5" s="1">
-        <f ca="1">SUMIF(C5:C498,J5,D5:D63)</f>
-        <v>5950</v>
+        <f ca="1">SUMIF(C5:C499,J5,D5:D63)</f>
+        <v>6085</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>99.166666666666671</v>
+        <v>101.41666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1097,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="K6" s="10">
-        <f ca="1">SUMIF(C6:C499,J6,D6:D64)</f>
+        <f ca="1">SUMIF(C6:C500,J6,D6:D64)</f>
         <v>3150</v>
       </c>
       <c r="L6" s="8">
@@ -4241,17 +4249,17 @@
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="2">
-        <v>44171</v>
+      <c r="A216" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D216" s="1">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="E216" s="1"/>
     </row>
@@ -4260,13 +4268,13 @@
         <v>44171</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D217" s="1">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E217" s="1"/>
     </row>
@@ -4275,13 +4283,13 @@
         <v>44171</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D218" s="1">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="E218" s="1"/>
     </row>
@@ -4290,10 +4298,10 @@
         <v>44171</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D219" s="1">
         <v>140</v>
@@ -4305,10 +4313,10 @@
         <v>44171</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D220" s="1">
         <v>140</v>
@@ -4323,7 +4331,7 @@
         <v>85</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D221" s="1">
         <v>140</v>
@@ -4332,46 +4340,62 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>44172</v>
+        <v>44171</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D222" s="1">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D223" s="1">
+        <v>42</v>
+      </c>
+      <c r="E223" s="1"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
         <v>44173</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B224" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C223" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D223" s="1">
+      <c r="C224" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D224" s="1">
         <v>45</v>
       </c>
-      <c r="E223" s="1"/>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" s="1"/>
-      <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
-      <c r="D224" s="1"/>
       <c r="E224" s="1"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A225" s="1"/>
-      <c r="B225" s="1"/>
-      <c r="C225" s="1"/>
-      <c r="D225" s="1"/>
+      <c r="A225" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D225" s="1">
+        <v>135</v>
+      </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -9218,13 +9242,20 @@
       <c r="D917" s="1"/>
       <c r="E917" s="1"/>
     </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A918" s="1"/>
+      <c r="B918" s="1"/>
+      <c r="C918" s="1"/>
+      <c r="D918" s="1"/>
+      <c r="E918" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C135 C137:C145 C147:C917" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C135 C137:C145 C147:C918">
       <formula1>$J$3:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -9366,18 +9397,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9399,14 +9430,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64438902-043F-48CD-B7EF-38455F47513D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -9420,4 +9443,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
implementatie van inventory, datalaag en domeinlaag except voor stock hiervoor zijn nog vragen + logboek
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar\Documents\School\Projectwerk\projectwerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0E60D-00F2-47E6-AF8D-01FF1C07AD1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85EE77D-3A58-4F85-941F-31E663D6D213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="140">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>sql script inventory</t>
+  </si>
+  <si>
+    <t>Werksessie inventory</t>
+  </si>
+  <si>
+    <t>Implementatie stock, aanmaken alles voor verkoop en aankoop</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H254" sqref="H254"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I262" sqref="I262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,11 +1109,11 @@
       </c>
       <c r="K4" s="1">
         <f ca="1">SUMIF(C4:C497,J4,D4:D62)</f>
-        <v>3750</v>
+        <v>3810</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" ref="L4:L6" ca="1" si="0">K4/60</f>
-        <v>62.5</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1155,11 +1161,11 @@
       </c>
       <c r="K6" s="10">
         <f ca="1">SUMIF(C6:C499,J6,D6:D64)</f>
-        <v>3745</v>
+        <v>4015</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>62.416666666666664</v>
+        <v>66.916666666666671</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4958,24 +4964,48 @@
       <c r="E259" s="1"/>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A260" s="1"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
+      <c r="A260" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D260" s="1">
+        <v>60</v>
+      </c>
       <c r="E260" s="1"/>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="1"/>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
-      <c r="D261" s="1"/>
+      <c r="A261" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D261" s="1">
+        <v>60</v>
+      </c>
       <c r="E261" s="1"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="1"/>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="1"/>
+      <c r="A262" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D262" s="1">
+        <v>210</v>
+      </c>
       <c r="E262" s="1"/>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Repo's + managers aangemaakt voor stock (nog niet getest)
</commit_message>
<xml_diff>
--- a/Logboek Team B2.xlsx
+++ b/Logboek Team B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lieke\OneDrive\scool\projectwerk inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59773B00-7428-49A3-8656-2A1F17AE3421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E49C5FE-5182-407B-A9CE-E5A73F1847AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23016" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="146">
   <si>
     <t>Logboek Team B2</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>Geprobeert om repos aan te maken voor Stock</t>
+  </si>
+  <si>
+    <t>Call met Lector</t>
+  </si>
+  <si>
+    <t>Repo's + managers aangemaakt voor stock (nog niet getest)</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1032,7 @@
   <dimension ref="A1:L917"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A259" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E268" sqref="E268"/>
+      <selection activeCell="D272" sqref="D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,11 +1127,11 @@
       </c>
       <c r="K4" s="1">
         <f ca="1">SUMIF(C4:C497,J4,D4:D62)</f>
-        <v>4040</v>
+        <v>4225</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" ref="L4:L6" ca="1" si="0">K4/60</f>
-        <v>67.333333333333329</v>
+        <v>70.416666666666671</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1147,11 +1153,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">SUMIF(C5:C498,J5,D5:D63)</f>
-        <v>6454</v>
+        <v>6484</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>107.56666666666666</v>
+        <v>108.06666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1173,11 +1179,11 @@
       </c>
       <c r="K6" s="10">
         <f ca="1">SUMIF(C6:C499,J6,D6:D64)</f>
-        <v>4065</v>
+        <v>4115</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>67.75</v>
+        <v>68.583333333333329</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -5111,31 +5117,63 @@
       <c r="E268" s="1"/>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A269" s="1"/>
-      <c r="B269" s="1"/>
-      <c r="C269" s="1"/>
-      <c r="D269" s="1"/>
+      <c r="A269" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D269" s="1">
+        <v>30</v>
+      </c>
       <c r="E269" s="1"/>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A270" s="1"/>
-      <c r="B270" s="1"/>
-      <c r="C270" s="1"/>
-      <c r="D270" s="1"/>
+      <c r="A270" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D270" s="1">
+        <v>50</v>
+      </c>
       <c r="E270" s="1"/>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A271" s="1"/>
-      <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
-      <c r="D271" s="1"/>
+      <c r="A271" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D271" s="1">
+        <v>50</v>
+      </c>
       <c r="E271" s="1"/>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A272" s="1"/>
-      <c r="B272" s="1"/>
-      <c r="C272" s="1"/>
-      <c r="D272" s="1"/>
+      <c r="A272" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D272" s="1">
+        <v>135</v>
+      </c>
       <c r="E272" s="1"/>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -9669,6 +9707,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA536D067EBDB642ACF72D467B71E2D5" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c3fcb91d1d9e32f823c02d5b2d9c9748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dd383423-36ee-428e-84ea-29af631fe386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9367320e87f463bd73a8985c785fc15e" ns3:_="">
     <xsd:import namespace="dd383423-36ee-428e-84ea-29af631fe386"/>
@@ -9800,35 +9853,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9850,9 +9878,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B4B5E02-53ED-4909-B0EA-30D7E8105257}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4EC5CCD-8AF0-4181-8080-8D23C7C643E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dd383423-36ee-428e-84ea-29af631fe386"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>